<commit_message>
Database updates; added many covers.
</commit_message>
<xml_diff>
--- a/data/PubFix.xlsx
+++ b/data/PubFix.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10040" yWindow="460" windowWidth="13120" windowHeight="16240" tabRatio="500"/>
+    <workbookView xWindow="9320" yWindow="460" windowWidth="13120" windowHeight="16240" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -860,9 +860,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E102"/>
+  <dimension ref="A1:E101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:C102"/>
     </sheetView>
   </sheetViews>
@@ -881,101 +881,86 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B3">
-        <v>24</v>
+        <v>3018</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="B4">
-        <v>54</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>172</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B5">
-        <v>67</v>
+        <v>113</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>45</v>
+        <v>88</v>
       </c>
       <c r="B6">
-        <v>225</v>
+        <v>2585</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>46</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7">
-        <v>278</v>
+        <v>49</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="B8">
-        <v>462</v>
+        <v>1237</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B9">
-        <v>494</v>
+        <v>71</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>126</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>78</v>
+        <v>108</v>
       </c>
       <c r="B10">
-        <v>498</v>
+        <v>4584</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>144</v>
+        <v>165</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>72</v>
+        <v>45</v>
       </c>
       <c r="B11">
-        <v>539</v>
+        <v>225</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>138</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -991,90 +976,78 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B13">
-        <v>565</v>
+        <v>100</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>129</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B14">
-        <v>574</v>
+        <v>91</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>142</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>65</v>
+        <v>95</v>
       </c>
       <c r="B15">
-        <v>604</v>
+        <v>847</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>133</v>
+        <v>156</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B16">
-        <v>608</v>
+        <v>54</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>44</v>
+        <v>123</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="B17">
-        <v>617</v>
+        <v>3467</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="B18">
-        <v>637</v>
+        <v>7</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>167</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="B19">
-        <v>731</v>
+        <v>24</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B20">
-        <v>754</v>
+        <v>604</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>32</v>
@@ -1082,549 +1055,524 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="B21">
-        <v>771</v>
+        <v>3591</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B22">
-        <v>847</v>
+        <v>17</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>99</v>
+        <v>118</v>
       </c>
       <c r="B23">
-        <v>946</v>
+        <v>3211</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>106</v>
+        <v>117</v>
       </c>
       <c r="B24">
-        <v>1163</v>
+        <v>731</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B25">
-        <v>1173</v>
+        <v>28</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>155</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B26">
-        <v>1237</v>
+        <v>81</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>48</v>
+        <v>147</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>73</v>
+        <v>5</v>
       </c>
       <c r="B27">
-        <v>1663</v>
+        <v>3279</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>139</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>84</v>
+        <v>120</v>
       </c>
       <c r="B28">
-        <v>1792</v>
+        <v>54</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>150</v>
+        <v>172</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B29">
-        <v>1802</v>
+        <v>105</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>128</v>
+        <v>18</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>87</v>
+        <v>62</v>
       </c>
       <c r="B30">
-        <v>1825</v>
+        <v>2094</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>152</v>
+        <v>130</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>83</v>
+        <v>39</v>
       </c>
       <c r="B31">
-        <v>2053</v>
+        <v>462</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>149</v>
+        <v>40</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="B32">
-        <v>2094</v>
+        <v>3186</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B33">
-        <v>2123</v>
+        <v>51</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>137</v>
+        <v>18</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>9</v>
+        <v>116</v>
       </c>
       <c r="B34">
-        <v>2193</v>
+        <v>7696</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>10</v>
+        <v>169</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>114</v>
+        <v>84</v>
       </c>
       <c r="B35">
-        <v>2397</v>
+        <v>1792</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>168</v>
+        <v>150</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B36">
-        <v>2453</v>
+        <v>19</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>160</v>
+        <v>20</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B37">
-        <v>2576</v>
+        <v>97</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>158</v>
+        <v>18</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>115</v>
+        <v>59</v>
       </c>
       <c r="B38">
-        <v>2576</v>
+        <v>771</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>158</v>
+        <v>127</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B39">
-        <v>2585</v>
+        <v>52</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>153</v>
+        <v>18</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>79</v>
+        <v>43</v>
       </c>
       <c r="B40">
-        <v>2755</v>
+        <v>608</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>145</v>
+        <v>44</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="B41">
-        <v>3018</v>
+        <v>35</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>162</v>
+        <v>18</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B42">
-        <v>3071</v>
+        <v>2453</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>68</v>
+        <v>106</v>
       </c>
       <c r="B43">
-        <v>3186</v>
+        <v>1163</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>136</v>
+        <v>163</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B44">
-        <v>3211</v>
+        <v>121</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>171</v>
+        <v>18</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B45">
-        <v>3279</v>
+        <v>90</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>6</v>
+        <v>154</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B46">
-        <v>3375</v>
+        <v>89</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>67</v>
+        <v>3</v>
       </c>
       <c r="B47">
-        <v>3467</v>
+        <v>9377</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>135</v>
+        <v>4</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B48">
-        <v>3591</v>
+        <v>15</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>134</v>
+        <v>16</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B49">
-        <v>3731</v>
+        <v>55</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>148</v>
+        <v>124</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B50">
-        <v>4080</v>
+        <v>6667</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="B51">
-        <v>4161</v>
+        <v>278</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>122</v>
+        <v>22</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>75</v>
+        <v>11</v>
       </c>
       <c r="B52">
-        <v>4198</v>
+        <v>9368</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>141</v>
+        <v>12</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>108</v>
+        <v>75</v>
       </c>
       <c r="B53">
-        <v>4584</v>
+        <v>4198</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>165</v>
+        <v>141</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>23</v>
+        <v>109</v>
       </c>
       <c r="B54">
-        <v>5132</v>
+        <v>6607</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>24</v>
+        <v>166</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>27</v>
+        <v>58</v>
       </c>
       <c r="B55">
-        <v>5132</v>
+        <v>494</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>24</v>
+        <v>126</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>109</v>
+        <v>61</v>
       </c>
       <c r="B56">
-        <v>6607</v>
+        <v>565</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>166</v>
+        <v>129</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B57">
-        <v>6667</v>
+        <v>96</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>140</v>
+        <v>157</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B58">
-        <v>6888</v>
+        <v>80</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>38</v>
+        <v>146</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B59">
-        <v>7236</v>
+        <v>86</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>151</v>
+        <v>18</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>116</v>
+        <v>69</v>
       </c>
       <c r="B60">
-        <v>7696</v>
+        <v>2123</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>169</v>
+        <v>137</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B61">
-        <v>9368</v>
+        <v>33</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>3</v>
+        <v>85</v>
       </c>
       <c r="B62">
-        <v>9377</v>
+        <v>7236</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>4</v>
+        <v>151</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>1</v>
+        <v>103</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>7</v>
+        <v>87</v>
+      </c>
+      <c r="B64">
+        <v>1825</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>8</v>
+        <v>152</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>15</v>
+        <v>56</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>17</v>
+        <v>77</v>
+      </c>
+      <c r="B66">
+        <v>4080</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>18</v>
+        <v>143</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>25</v>
+        <v>53</v>
+      </c>
+      <c r="B68">
+        <v>4161</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>18</v>
+        <v>122</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>26</v>
+        <v>99</v>
+      </c>
+      <c r="B69">
+        <v>946</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>18</v>
+        <v>159</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>28</v>
+        <v>82</v>
+      </c>
+      <c r="B70">
+        <v>3731</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>29</v>
+        <v>148</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B72">
+        <v>617</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>33</v>
+        <v>102</v>
+      </c>
+      <c r="B73">
+        <v>3071</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>18</v>
+        <v>161</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>18</v>
@@ -1632,39 +1580,51 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>35</v>
+        <v>73</v>
+      </c>
+      <c r="B75">
+        <v>1663</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>18</v>
+        <v>139</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>36</v>
+        <v>41</v>
+      </c>
+      <c r="B76">
+        <v>67</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>49</v>
+        <v>63</v>
+      </c>
+      <c r="B77">
+        <v>754</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>50</v>
+        <v>131</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>51</v>
+        <v>78</v>
+      </c>
+      <c r="B78">
+        <v>498</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>18</v>
+        <v>144</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>52</v>
+        <v>26</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>18</v>
@@ -1672,39 +1632,48 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>54</v>
+        <v>112</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>123</v>
+        <v>18</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>55</v>
+        <v>79</v>
+      </c>
+      <c r="B81">
+        <v>2755</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>124</v>
+        <v>145</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>56</v>
+        <v>60</v>
+      </c>
+      <c r="B82">
+        <v>1802</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>18</v>
+        <v>128</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
+      </c>
+      <c r="B83">
+        <v>539</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>29</v>
+        <v>138</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>71</v>
+        <v>25</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>18</v>
@@ -1712,23 +1681,23 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
+      </c>
+      <c r="B85">
+        <v>2053</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>147</v>
+        <v>111</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>86</v>
+        <v>119</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>18</v>
@@ -1736,7 +1705,7 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>18</v>
@@ -1744,113 +1713,144 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>90</v>
+        <v>76</v>
+      </c>
+      <c r="B89">
+        <v>574</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>91</v>
+        <v>94</v>
+      </c>
+      <c r="B90">
+        <v>1173</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>18</v>
+        <v>155</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>92</v>
+        <v>37</v>
+      </c>
+      <c r="B91">
+        <v>6888</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>93</v>
+        <v>1</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>96</v>
+        <v>9</v>
+      </c>
+      <c r="B93">
+        <v>2193</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>157</v>
+        <v>10</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>97</v>
+        <v>23</v>
+      </c>
+      <c r="B94">
+        <v>5132</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
-        <v>100</v>
+        <v>27</v>
+      </c>
+      <c r="B95">
+        <v>5132</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
-        <v>103</v>
+        <v>110</v>
+      </c>
+      <c r="B96">
+        <v>637</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>18</v>
+        <v>167</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>105</v>
+        <v>98</v>
+      </c>
+      <c r="B97">
+        <v>2576</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>18</v>
+        <v>158</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>111</v>
+        <v>115</v>
+      </c>
+      <c r="B98">
+        <v>2576</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>112</v>
+        <v>30</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
-        <v>113</v>
+        <v>13</v>
+      </c>
+      <c r="B100">
+        <v>3375</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
-        <v>119</v>
+        <v>114</v>
+      </c>
+      <c r="B101">
+        <v>2397</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A102" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C102" s="1" t="s">
-        <v>18</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>
   <sortState ref="A3:C102">
-    <sortCondition ref="B3:B102"/>
+    <sortCondition ref="A3:A102"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>